<commit_message>
Data overview and variable documentation modified
</commit_message>
<xml_diff>
--- a/data/out/Variable_Documentation.xlsx
+++ b/data/out/Variable_Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebbamark/Documents/GitHub/break_scoping/data/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25989C45-B0C2-A642-AF34-B0A5368C0E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B727FA6E-9506-2E44-AD05-9702929DF6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CF581617-EF99-AC40-8A27-9142B70BDDA1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{CF581617-EF99-AC40-8A27-9142B70BDDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="221">
   <si>
     <t>country</t>
   </si>
@@ -687,32 +687,38 @@
     <t>Generation- Geothermal, Biomass and Other*</t>
   </si>
   <si>
-    <t>CO2 emissions from electricity, measured in tonnes of 
+    <t>International Energy Agency (IEA)</t>
+  </si>
+  <si>
+    <t>International Energy Agency. (2021). International Energy Agency Greenhouse Gas Emissions from Energy, 1751-2020. [data collection]. 13th Edition. UK Data Service. SN: 5181, DOI: 10.5257/iea/co2/2021</t>
+  </si>
+  <si>
+    <t>https://stats2.digitalresources.jisc.ac.uk/metadata/IEA/gge/Greenhouse_Gas_Emissions_from_Energy_documentation.pdf</t>
+  </si>
+  <si>
+    <t>Electricity and heat production contains the sum of emissions from electricity production, combined heat and power plants and heat plants. It is the sum of main activity producers and autoproducers. Emissions from own on-site use of fuel are included.</t>
+  </si>
+  <si>
+    <t>Emissions from electricity and heat production per capita</t>
+  </si>
+  <si>
+    <t>Emissions from electricity and heat production</t>
+  </si>
+  <si>
+    <t>Fossil fuel consumprtion per capita (unit unknown)</t>
+  </si>
+  <si>
+    <t>Emissions are measured in tonnes of carbon dioxide equivalents (CO2eq). Thismeans non-CO2 gases are weighted by the amount of warming theycause over a 100-year timescale.</t>
+  </si>
+  <si>
+    <t>CO2 emissions from electricity, measured in thousand tonnes of 
 carbon dioxide-equivalents.</t>
   </si>
   <si>
-    <t>International Energy Agency (IEA)</t>
-  </si>
-  <si>
-    <t>International Energy Agency. (2021). International Energy Agency Greenhouse Gas Emissions from Energy, 1751-2020. [data collection]. 13th Edition. UK Data Service. SN: 5181, DOI: 10.5257/iea/co2/2021</t>
-  </si>
-  <si>
-    <t>https://stats2.digitalresources.jisc.ac.uk/metadata/IEA/gge/Greenhouse_Gas_Emissions_from_Energy_documentation.pdf</t>
-  </si>
-  <si>
-    <t>Electricity and heat production contains the sum of emissions from electricity production, combined heat and power plants and heat plants. It is the sum of main activity producers and autoproducers. Emissions from own on-site use of fuel are included.</t>
-  </si>
-  <si>
-    <t>Emissions from electricity and heat production per capita</t>
-  </si>
-  <si>
-    <t>Emissions are measured in carbon dioxide equivalents (CO2eq). Thismeans non-CO2 gases are weighted by the amount of warming theycause over a 100-year timescale.</t>
-  </si>
-  <si>
-    <t>Emissions from electricity and heat production</t>
-  </si>
-  <si>
-    <t>Fossil fuel consumprtion per capita (unit unknown)</t>
+    <t>emissions_elec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emissions from electricity OECD countries, </t>
   </si>
 </sst>
 </file>
@@ -871,12 +877,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1194,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4165AE-E18E-EB45-8B7A-EE22749D419D}">
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,17 +1255,17 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="182" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>210</v>
+      <c r="B4" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="C4" t="s">
         <v>197</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>198</v>
       </c>
       <c r="E4" t="s">
@@ -1413,21 +1421,21 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>200</v>
       </c>
       <c r="C18" t="s">
         <v>195</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1441,7 +1449,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1458,7 +1466,7 @@
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>201</v>
       </c>
       <c r="C21" t="s">
@@ -1721,15 +1729,15 @@
         <v>94</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="C43" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="E43" s="12" t="s">
         <v>196</v>
       </c>
     </row>
@@ -1858,7 +1866,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2525,7 +2533,7 @@
         <v>19</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C91" t="s">
         <v>156</v>
@@ -2553,16 +2561,16 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C93" t="s">
+        <v>210</v>
+      </c>
+      <c r="E93" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E93" s="13" t="s">
+      <c r="F93" t="s">
         <v>212</v>
-      </c>
-      <c r="F93" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2570,45 +2578,53 @@
         <v>96</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C94" t="s">
+        <v>210</v>
+      </c>
+      <c r="E94" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E94" s="13" t="s">
+      <c r="F94" t="s">
         <v>212</v>
       </c>
-      <c r="F94" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="A95" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C95" t="s">
+        <v>68</v>
+      </c>
+      <c r="E95" s="12"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="1"/>
-      <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
@@ -2636,10 +2652,10 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
+      <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
-      <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
@@ -2728,11 +2744,16 @@
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="2"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1"/>
+      <c r="B129" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E93" r:id="rId1" display="http://doi.org/10.5257/iea/co2/2021" xr:uid="{F4F818D8-99E1-6847-8B95-D3C0249FDA68}"/>
     <hyperlink ref="E94" r:id="rId2" display="http://doi.org/10.5257/iea/co2/2021" xr:uid="{B338BF4B-F3D6-D147-B41A-1168CF12743F}"/>
+    <hyperlink ref="E43" r:id="rId3" location="annual-greenhouse-gas-emissions-by-sector" xr:uid="{C9AA8D8F-30EC-CD4D-BCE6-4D8942B90195}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>